<commit_message>
updates for the new week
</commit_message>
<xml_diff>
--- a/Notes/DS Hour Tracker.xlsx
+++ b/Notes/DS Hour Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DCWitten\Documents\Personal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5F6459-D6BB-4B25-BBD4-05FED740EFA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9EF2D3-5253-413D-BC45-1151582D0028}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11630" xr2:uid="{301E6A16-650B-4F11-AF02-EFFF9A664987}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{301E6A16-650B-4F11-AF02-EFFF9A664987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>Hour Tracking Spreadsheet</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Total</t>
   </si>
@@ -414,21 +411,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8B0DA4-E459-486D-9786-16D34BE2C0CA}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43675</v>
       </c>
@@ -436,7 +435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43682</v>
       </c>
@@ -444,7 +443,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43689</v>
       </c>
@@ -452,7 +451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43696</v>
       </c>
@@ -460,7 +459,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43703</v>
       </c>
@@ -468,7 +467,7 @@
         <v>20.75</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43710</v>
       </c>
@@ -476,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43717</v>
       </c>
@@ -484,7 +483,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43724</v>
       </c>
@@ -492,7 +491,7 @@
         <v>7.25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43731</v>
       </c>
@@ -500,7 +499,7 @@
         <v>20.75</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43738</v>
       </c>
@@ -508,7 +507,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43745</v>
       </c>
@@ -516,7 +515,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43752</v>
       </c>
@@ -524,7 +523,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43759</v>
       </c>
@@ -532,7 +531,7 @@
         <v>16.75</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43766</v>
       </c>
@@ -540,7 +539,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43773</v>
       </c>
@@ -548,7 +547,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43780</v>
       </c>
@@ -556,7 +555,7 @@
         <v>9.25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43787</v>
       </c>
@@ -564,7 +563,7 @@
         <v>16.25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43794</v>
       </c>
@@ -572,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43801</v>
       </c>
@@ -580,7 +579,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43808</v>
       </c>
@@ -588,7 +587,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43815</v>
       </c>
@@ -596,7 +595,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43822</v>
       </c>
@@ -604,7 +603,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43829</v>
       </c>
@@ -612,7 +611,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43836</v>
       </c>
@@ -620,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43843</v>
       </c>
@@ -628,30 +627,38 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="6">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>43850</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>43857</v>
+      </c>
+      <c r="B28" s="7">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="3">
+        <f>SUM(B2:B28)</f>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="3">
-        <f>SUM(B2:B27)</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29" s="3">
-        <f>B28/COUNT(B2:B27)</f>
-        <v>11.538461538461538</v>
+      <c r="B30" s="3">
+        <f>B29/COUNT(B2:B28)</f>
+        <v>11.222222222222221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>